<commit_message>
Datetime cols now display time only
</commit_message>
<xml_diff>
--- a/src/dataout/18max_pip_mvmts.xlsx
+++ b/src/dataout/18max_pip_mvmts.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viclee/Developer/_gbfx/fx-research/edge_research/dataout/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/viclee/Developer/_gbfx/fx-research/src/dataout/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04C1C54D-C2FA-F642-8555-351EDF98D5BA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23256E12-B45E-C746-95EE-024472B9909A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="max_pip_mvmts" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
   <dimension ref="A1:W260"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>